<commit_message>
created new url def, new neear template
</commit_message>
<xml_diff>
--- a/static/data/2012portfolio_leslie1.xlsx
+++ b/static/data/2012portfolio_leslie1.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="2012portfolio_leslie2.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
   <si>
     <t>NEEAR</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Construction</t>
   </si>
   <si>
-    <t>Vimeo</t>
-  </si>
-  <si>
     <t>SonyNex</t>
   </si>
   <si>
@@ -175,6 +172,21 @@
   </si>
   <si>
     <t>About [12]</t>
+  </si>
+  <si>
+    <t>http://farm8.staticflickr.com/7200/6978558121_3f3c2159c1.jpg</t>
+  </si>
+  <si>
+    <t>http://network.aia.org/AIA/Blogs/BlogViewer/?BlogKey=8538827c-53b4-4fc8-b5ae-8a9d6b2c3463</t>
+  </si>
+  <si>
+    <t>http://farm8.staticflickr.com/7127/6942702324_9930c10893.jpg</t>
+  </si>
+  <si>
+    <t>Montages</t>
+  </si>
+  <si>
+    <t>http://farm5.staticflickr.com/4050/4318703671_f54767fa09.jpg</t>
   </si>
 </sst>
 </file>
@@ -184,10 +196,26 @@
   <numFmts count="1">
     <numFmt numFmtId="165" formatCode="m/d/yyyy;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -210,8 +238,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -220,7 +250,9 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -552,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -568,54 +600,54 @@
     <col min="8" max="8" width="20.83203125" customWidth="1"/>
     <col min="9" max="9" width="19.33203125" customWidth="1"/>
     <col min="10" max="10" width="36.6640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="32.6640625" customWidth="1"/>
+    <col min="11" max="11" width="32.6640625" style="2" customWidth="1"/>
     <col min="12" max="12" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K1" t="s">
-        <v>30</v>
-      </c>
       <c r="L1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="30">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -636,27 +668,27 @@
         <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I2" t="s">
         <v>3</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="L2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="30">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -671,30 +703,33 @@
         <v>39586</v>
       </c>
       <c r="F3" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="G3">
         <v>20</v>
       </c>
       <c r="H3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" t="s">
         <v>12</v>
       </c>
-      <c r="I3" t="s">
-        <v>3</v>
-      </c>
       <c r="J3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="L3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="30">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -709,36 +744,36 @@
         <v>39586</v>
       </c>
       <c r="F4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G4">
         <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I4" t="s">
         <v>3</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" ht="30">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
         <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
       </c>
       <c r="D5" s="1">
         <v>39305</v>
@@ -753,27 +788,30 @@
         <v>200</v>
       </c>
       <c r="H5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I5" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="L5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
         <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
       </c>
       <c r="D6" s="1">
         <v>39398</v>
@@ -782,33 +820,33 @@
         <v>39404</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G6">
         <v>200</v>
       </c>
       <c r="H6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I6" t="s">
         <v>3</v>
       </c>
       <c r="L6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" ht="45">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
         <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
       </c>
       <c r="D7" s="1">
         <v>39416</v>
@@ -817,33 +855,36 @@
         <v>39416</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7">
         <v>200</v>
       </c>
       <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" t="s">
         <v>12</v>
       </c>
-      <c r="I7" t="s">
-        <v>13</v>
+      <c r="K7" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="L7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
         <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
       </c>
       <c r="D8" s="1">
         <v>37376</v>
@@ -852,33 +893,33 @@
         <v>38472</v>
       </c>
       <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
         <v>16</v>
       </c>
-      <c r="G8" t="s">
-        <v>17</v>
-      </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I8" t="s">
         <v>3</v>
       </c>
       <c r="L8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="30">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
         <v>36</v>
       </c>
-      <c r="M8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="1">
         <v>36346</v>
@@ -887,29 +928,33 @@
         <v>36664</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G9">
         <v>40</v>
       </c>
       <c r="H9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I9" t="s">
         <v>3</v>
       </c>
       <c r="J9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L9" t="s">
         <v>42</v>
       </c>
-      <c r="L9" t="s">
-        <v>43</v>
-      </c>
       <c r="M9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Setting up project id in csv to filter.  Mohit helped with setting up projects template.
Leslie worked on instantiating project_id - and creating a projected
method
</commit_message>
<xml_diff>
--- a/static/data/2012portfolio_leslie1.xlsx
+++ b/static/data/2012portfolio_leslie1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
   <si>
     <t>NEEAR</t>
   </si>
@@ -187,6 +187,24 @@
   </si>
   <si>
     <t>http://farm5.staticflickr.com/4050/4318703671_f54767fa09.jpg</t>
+  </si>
+  <si>
+    <t>is_public</t>
+  </si>
+  <si>
+    <t>project_id</t>
+  </si>
+  <si>
+    <t>neear</t>
+  </si>
+  <si>
+    <t>aia_crafting_the_future</t>
+  </si>
+  <si>
+    <t>ajo_artisan_lofts</t>
+  </si>
+  <si>
+    <t>building_with_bamboo_desert</t>
   </si>
 </sst>
 </file>
@@ -238,8 +256,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -250,9 +272,13 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -582,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -602,9 +628,10 @@
     <col min="10" max="10" width="36.6640625" style="2" customWidth="1"/>
     <col min="11" max="11" width="32.6640625" style="2" customWidth="1"/>
     <col min="12" max="12" width="21.83203125" customWidth="1"/>
+    <col min="13" max="13" width="19.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -644,8 +671,14 @@
       <c r="M1" t="s">
         <v>50</v>
       </c>
+      <c r="N1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" ht="30">
+    <row r="2" spans="1:15" ht="30">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -685,8 +718,14 @@
       <c r="M2" t="s">
         <v>46</v>
       </c>
+      <c r="N2" t="s">
+        <v>58</v>
+      </c>
+      <c r="O2" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" ht="30">
+    <row r="3" spans="1:15" ht="30">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -726,8 +765,14 @@
       <c r="M3" t="s">
         <v>46</v>
       </c>
+      <c r="N3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O3" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" ht="30">
+    <row r="4" spans="1:15" ht="30">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -764,8 +809,14 @@
       <c r="M4" t="s">
         <v>46</v>
       </c>
+      <c r="N4" t="s">
+        <v>58</v>
+      </c>
+      <c r="O4" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" ht="30">
+    <row r="5" spans="1:15" ht="30">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -802,8 +853,14 @@
       <c r="M5" t="s">
         <v>47</v>
       </c>
+      <c r="N5" t="s">
+        <v>59</v>
+      </c>
+      <c r="O5" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -837,8 +894,14 @@
       <c r="M6" t="s">
         <v>47</v>
       </c>
+      <c r="N6" t="s">
+        <v>59</v>
+      </c>
+      <c r="O6" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" ht="45">
+    <row r="7" spans="1:15" ht="45">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -875,8 +938,14 @@
       <c r="M7" t="s">
         <v>47</v>
       </c>
+      <c r="N7" t="s">
+        <v>59</v>
+      </c>
+      <c r="O7" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -910,8 +979,14 @@
       <c r="M8" t="s">
         <v>48</v>
       </c>
+      <c r="N8" t="s">
+        <v>60</v>
+      </c>
+      <c r="O8" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:13" ht="30">
+    <row r="9" spans="1:15" ht="30">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -950,6 +1025,12 @@
       </c>
       <c r="M9" t="s">
         <v>49</v>
+      </c>
+      <c r="N9" t="s">
+        <v>61</v>
+      </c>
+      <c r="O9" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed Index to just render 1 image at a time
Move {{project.image_urls}} to allproject.html
</commit_message>
<xml_diff>
--- a/static/data/2012portfolio_leslie1.xlsx
+++ b/static/data/2012portfolio_leslie1.xlsx
@@ -180,9 +180,6 @@
     <t>http://network.aia.org/AIA/Blogs/BlogViewer/?BlogKey=8538827c-53b4-4fc8-b5ae-8a9d6b2c3463</t>
   </si>
   <si>
-    <t>http://farm8.staticflickr.com/7127/6942702324_9930c10893.jpg</t>
-  </si>
-  <si>
     <t>Montages</t>
   </si>
   <si>
@@ -205,6 +202,9 @@
   </si>
   <si>
     <t>building_with_bamboo_desert</t>
+  </si>
+  <si>
+    <t>http://farm6.staticflickr.com/5325/7088736843_0028cabf61.jpg</t>
   </si>
 </sst>
 </file>
@@ -610,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -672,10 +672,10 @@
         <v>50</v>
       </c>
       <c r="N1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="30">
@@ -719,7 +719,7 @@
         <v>46</v>
       </c>
       <c r="N2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O2" t="b">
         <v>1</v>
@@ -742,7 +742,7 @@
         <v>39586</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G3">
         <v>20</v>
@@ -757,7 +757,7 @@
         <v>18</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="L3" t="s">
         <v>32</v>
@@ -766,7 +766,7 @@
         <v>46</v>
       </c>
       <c r="N3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O3" t="b">
         <v>1</v>
@@ -810,7 +810,7 @@
         <v>46</v>
       </c>
       <c r="N4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O4" t="b">
         <v>1</v>
@@ -854,7 +854,7 @@
         <v>47</v>
       </c>
       <c r="N5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O5" t="b">
         <v>1</v>
@@ -895,7 +895,7 @@
         <v>47</v>
       </c>
       <c r="N6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O6" t="b">
         <v>1</v>
@@ -939,7 +939,7 @@
         <v>47</v>
       </c>
       <c r="N7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O7" t="b">
         <v>1</v>
@@ -980,7 +980,7 @@
         <v>48</v>
       </c>
       <c r="N8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O8" t="b">
         <v>1</v>
@@ -1018,7 +1018,7 @@
         <v>41</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L9" t="s">
         <v>42</v>
@@ -1027,7 +1027,7 @@
         <v>49</v>
       </c>
       <c r="N9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O9" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Tried to tie project.html into project, More HTML Index work
Experimented with div's in index {% for statement %}
</commit_message>
<xml_diff>
--- a/static/data/2012portfolio_leslie1.xlsx
+++ b/static/data/2012portfolio_leslie1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="63">
   <si>
     <t>NEEAR</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Construction</t>
   </si>
   <si>
-    <t>SonyNex</t>
-  </si>
-  <si>
     <t>Knowledge Scholar</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>Navigating an Educational Experience by Augmenting our Reality</t>
   </si>
   <si>
-    <t>http://farm8.staticflickr.com/7217/7250501718_87584a49bb.jpg</t>
-  </si>
-  <si>
     <t>Organization_category [0]</t>
   </si>
   <si>
@@ -205,6 +199,15 @@
   </si>
   <si>
     <t>http://farm6.staticflickr.com/5325/7088736843_0028cabf61.jpg</t>
+  </si>
+  <si>
+    <t>http://farm9.staticflickr.com/8146/7469445394_ab04faaa6f.jpg</t>
+  </si>
+  <si>
+    <t>http://farm8.staticflickr.com/7251/7469566482_a8e3a40df8.jpg</t>
+  </si>
+  <si>
+    <t>SonyNex: Photoshop</t>
   </si>
 </sst>
 </file>
@@ -610,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -633,54 +636,54 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>25</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="L1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="30">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -695,31 +698,31 @@
         <v>39586</v>
       </c>
       <c r="F2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G2">
         <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I2" t="s">
         <v>3</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="L2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O2" t="b">
         <v>1</v>
@@ -727,7 +730,7 @@
     </row>
     <row r="3" spans="1:15" ht="30">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -742,31 +745,31 @@
         <v>39586</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G3">
         <v>20</v>
       </c>
       <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
         <v>11</v>
       </c>
-      <c r="I3" t="s">
-        <v>12</v>
-      </c>
       <c r="J3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O3" t="b">
         <v>1</v>
@@ -774,7 +777,7 @@
     </row>
     <row r="4" spans="1:15" ht="30">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -789,28 +792,31 @@
         <v>39586</v>
       </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="G4">
         <v>20</v>
       </c>
       <c r="H4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
         <v>11</v>
       </c>
-      <c r="I4" t="s">
-        <v>3</v>
-      </c>
       <c r="J4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="L4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O4" t="b">
         <v>1</v>
@@ -818,13 +824,13 @@
     </row>
     <row r="5" spans="1:15" ht="30">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
         <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
       </c>
       <c r="D5" s="1">
         <v>39305</v>
@@ -839,22 +845,22 @@
         <v>200</v>
       </c>
       <c r="H5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="M5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="N5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="O5" t="b">
         <v>1</v>
@@ -862,13 +868,13 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
         <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
       </c>
       <c r="D6" s="1">
         <v>39398</v>
@@ -877,25 +883,25 @@
         <v>39404</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G6">
         <v>200</v>
       </c>
       <c r="H6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I6" t="s">
         <v>3</v>
       </c>
       <c r="L6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="N6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="O6" t="b">
         <v>1</v>
@@ -903,13 +909,13 @@
     </row>
     <row r="7" spans="1:15" ht="45">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
         <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
       </c>
       <c r="D7" s="1">
         <v>39416</v>
@@ -918,28 +924,28 @@
         <v>39416</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G7">
         <v>200</v>
       </c>
       <c r="H7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" t="s">
         <v>11</v>
       </c>
-      <c r="I7" t="s">
-        <v>12</v>
-      </c>
       <c r="K7" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="N7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="O7" t="b">
         <v>1</v>
@@ -947,13 +953,13 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
         <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
       </c>
       <c r="D8" s="1">
         <v>37376</v>
@@ -962,25 +968,25 @@
         <v>38472</v>
       </c>
       <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
         <v>15</v>
       </c>
-      <c r="G8" t="s">
-        <v>16</v>
-      </c>
       <c r="H8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I8" t="s">
         <v>3</v>
       </c>
       <c r="L8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="N8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="O8" t="b">
         <v>1</v>
@@ -988,13 +994,13 @@
     </row>
     <row r="9" spans="1:15" ht="30">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
         <v>36</v>
-      </c>
-      <c r="C9" t="s">
-        <v>38</v>
       </c>
       <c r="D9" s="1">
         <v>36346</v>
@@ -1003,31 +1009,31 @@
         <v>36664</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G9">
         <v>40</v>
       </c>
       <c r="H9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I9" t="s">
         <v>3</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O9" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Tied get_construction_projects def to index
Mohit helped.
</commit_message>
<xml_diff>
--- a/static/data/2012portfolio_leslie1.xlsx
+++ b/static/data/2012portfolio_leslie1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="69">
   <si>
     <t>NEEAR</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Japan</t>
   </si>
   <si>
-    <t>Word processing</t>
-  </si>
-  <si>
     <t>Berkeley</t>
   </si>
   <si>
@@ -208,6 +205,27 @@
   </si>
   <si>
     <t>SonyNex: Photoshop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winning Grant Proposal for Inaugral AIA Knowledge Scholar  </t>
+  </si>
+  <si>
+    <t>Reflection blogs and How is [it] Done Well Knowledge Scholar Project</t>
+  </si>
+  <si>
+    <t>Implimented How is [it] Done Well in Japan</t>
+  </si>
+  <si>
+    <t>Sketching</t>
+  </si>
+  <si>
+    <t>http://farm7.staticflickr.com/6119/6422285629_fff812d248.jpg</t>
+  </si>
+  <si>
+    <t>Award winning Historic Preservation image for Ajo Artisan Lofts</t>
+  </si>
+  <si>
+    <t>http://farm8.staticflickr.com/7169/6742591635_54ffc92751.jpg</t>
   </si>
 </sst>
 </file>
@@ -259,8 +277,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -275,13 +295,15 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -613,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -636,54 +658,54 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="L1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="30">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -698,31 +720,31 @@
         <v>39586</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2">
         <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I2" t="s">
         <v>3</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O2" t="b">
         <v>1</v>
@@ -730,7 +752,7 @@
     </row>
     <row r="3" spans="1:15" ht="30">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -745,31 +767,31 @@
         <v>39586</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G3">
         <v>20</v>
       </c>
       <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
         <v>10</v>
       </c>
-      <c r="I3" t="s">
-        <v>11</v>
-      </c>
       <c r="J3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O3" t="b">
         <v>1</v>
@@ -777,7 +799,7 @@
     </row>
     <row r="4" spans="1:15" ht="30">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -792,31 +814,31 @@
         <v>39586</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G4">
         <v>20</v>
       </c>
       <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
         <v>10</v>
       </c>
-      <c r="I4" t="s">
-        <v>11</v>
-      </c>
       <c r="J4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O4" t="b">
         <v>1</v>
@@ -824,7 +846,7 @@
     </row>
     <row r="5" spans="1:15" ht="30">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -845,30 +867,33 @@
         <v>200</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I5" t="s">
         <v>6</v>
       </c>
+      <c r="J5" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="K5" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" ht="30">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -883,7 +908,7 @@
         <v>39404</v>
       </c>
       <c r="F6" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="G6">
         <v>200</v>
@@ -892,16 +917,22 @@
         <v>8</v>
       </c>
       <c r="I6" t="s">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="L6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O6" t="b">
         <v>1</v>
@@ -909,7 +940,7 @@
     </row>
     <row r="7" spans="1:15" ht="45">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -924,42 +955,45 @@
         <v>39416</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G7">
         <v>200</v>
       </c>
       <c r="H7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I7" t="s">
-        <v>11</v>
+        <v>3</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O7" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" ht="30">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
         <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
       </c>
       <c r="D8" s="1">
         <v>37376</v>
@@ -968,25 +1002,31 @@
         <v>38472</v>
       </c>
       <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
         <v>14</v>
       </c>
-      <c r="G8" t="s">
-        <v>15</v>
-      </c>
       <c r="H8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I8" t="s">
         <v>3</v>
       </c>
+      <c r="J8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="L8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O8" t="b">
         <v>1</v>
@@ -994,13 +1034,13 @@
     </row>
     <row r="9" spans="1:15" ht="30">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="1">
         <v>36346</v>
@@ -1009,31 +1049,31 @@
         <v>36664</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G9">
         <v>40</v>
       </c>
       <c r="H9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I9" t="s">
         <v>3</v>
       </c>
       <c r="J9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L9" t="s">
         <v>39</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L9" t="s">
-        <v>40</v>
-      </c>
       <c r="M9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O9" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Add comments to code, delete bySchool.html, chance csv files and css files to render website better.
</commit_message>
<xml_diff>
--- a/static/data/2012portfolio_leslie1.xlsx
+++ b/static/data/2012portfolio_leslie1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="0" windowWidth="25600" windowHeight="16940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="2012portfolio_leslie2.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="79">
   <si>
     <t>NEEAR</t>
   </si>
@@ -123,9 +123,6 @@
     <t>Building with Bamboo</t>
   </si>
   <si>
-    <t>Project Title [1] (char limit?)</t>
-  </si>
-  <si>
     <t xml:space="preserve">My Architecture final project </t>
   </si>
   <si>
@@ -226,6 +223,39 @@
   </si>
   <si>
     <t>http://farm8.staticflickr.com/7169/6742591635_54ffc92751.jpg</t>
+  </si>
+  <si>
+    <t>Teaching Assisstant for Resource and Metadata Course</t>
+  </si>
+  <si>
+    <t>Teaching</t>
+  </si>
+  <si>
+    <t>Teaching Assistant for Resource and Metadata Course</t>
+  </si>
+  <si>
+    <t>resource_metadata_course</t>
+  </si>
+  <si>
+    <t>During the conference we had time to sketch during our train and motor car rides throughout Japan.  This is a sketch that will be added to the How is [it] Done Well project.</t>
+  </si>
+  <si>
+    <t>http://farm8.staticflickr.com/7179/7005684653_1117b17580.jpg</t>
+  </si>
+  <si>
+    <t>To work through the user experience and understanding the layering of what needs to be buil: I worked with my team to finalize what needs to be done through montaging.</t>
+  </si>
+  <si>
+    <t>In 72 hours: I created a submission proposal for the AIA Committee on Design: Crafting the Future Conference.  I was highly influenced by my architecture past and finishing one year at UC Berkeley's School of Information.  I highlighted process: timeline: budget: and issues like privacy: adoption: etc.</t>
+  </si>
+  <si>
+    <t>Patrick Schmitz lead development architect for CollectionSpace: my summer internship taught the theory and practice of working with a client to move them to CollectionSpace: a Museum Content Management System.</t>
+  </si>
+  <si>
+    <t>project_title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Augmented Reality is dynamically flatening our physical 3-Dimensional world into 2-Dimension tablet Screen.  This image represents the work of photographing and understanding 180 into a flat representation.  </t>
   </si>
 </sst>
 </file>
@@ -233,7 +263,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -277,8 +307,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -290,20 +322,22 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -633,17 +667,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26.5" customWidth="1"/>
     <col min="2" max="2" width="25.5" customWidth="1"/>
-    <col min="3" max="3" width="60.5" customWidth="1"/>
+    <col min="3" max="3" width="140" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
@@ -661,9 +695,9 @@
         <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -691,16 +725,16 @@
         <v>26</v>
       </c>
       <c r="L1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="30">
@@ -710,7 +744,7 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1">
@@ -735,16 +769,16 @@
         <v>16</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L2" t="s">
         <v>29</v>
       </c>
       <c r="M2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O2" t="b">
         <v>1</v>
@@ -757,8 +791,8 @@
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
-        <v>1</v>
+      <c r="C3" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="D3" s="1">
         <v>39671</v>
@@ -767,7 +801,7 @@
         <v>39586</v>
       </c>
       <c r="F3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G3">
         <v>20</v>
@@ -782,16 +816,16 @@
         <v>16</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L3" t="s">
         <v>29</v>
       </c>
       <c r="M3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O3" t="b">
         <v>1</v>
@@ -804,8 +838,8 @@
       <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
-        <v>1</v>
+      <c r="C4" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="D4" s="1">
         <v>39398</v>
@@ -814,7 +848,7 @@
         <v>39586</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G4">
         <v>20</v>
@@ -829,16 +863,16 @@
         <v>16</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L4" t="s">
         <v>29</v>
       </c>
       <c r="M4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O4" t="b">
         <v>1</v>
@@ -846,46 +880,46 @@
     </row>
     <row r="5" spans="1:15" ht="30">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
+        <v>68</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="D5" s="1">
-        <v>39305</v>
+        <v>39465</v>
       </c>
       <c r="E5" s="1">
-        <v>39404</v>
+        <v>39586</v>
       </c>
       <c r="F5" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="G5">
-        <v>200</v>
+        <v>6</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="I5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="L5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M5" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="N5" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="O5" t="b">
         <v>1</v>
@@ -893,140 +927,140 @@
     </row>
     <row r="6" spans="1:15" ht="30">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
-        <v>5</v>
+      <c r="C6" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="D6" s="1">
-        <v>39398</v>
+        <v>39305</v>
       </c>
       <c r="E6" s="1">
         <v>39404</v>
       </c>
       <c r="F6" t="s">
-        <v>65</v>
+        <v>2</v>
       </c>
       <c r="G6">
         <v>200</v>
       </c>
       <c r="H6" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="I6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="L6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O6" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="45">
+    <row r="7" spans="1:15" ht="30">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
-        <v>5</v>
+      <c r="C7" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="D7" s="1">
-        <v>39416</v>
+        <v>39398</v>
       </c>
       <c r="E7" s="1">
-        <v>39416</v>
+        <v>39404</v>
       </c>
       <c r="F7" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="G7">
         <v>200</v>
       </c>
       <c r="H7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I7" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>63</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="L7" t="s">
         <v>31</v>
       </c>
       <c r="M7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O7" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="30">
+    <row r="8" spans="1:15" ht="45">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="D8" s="1">
-        <v>37376</v>
+        <v>39416</v>
       </c>
       <c r="E8" s="1">
-        <v>38472</v>
+        <v>39416</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" t="s">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>200</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="I8" t="s">
         <v>3</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="L8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="N8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O8" t="b">
         <v>1</v>
@@ -1034,48 +1068,95 @@
     </row>
     <row r="9" spans="1:15" ht="30">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>35</v>
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D9" s="1">
-        <v>36346</v>
+        <v>37376</v>
       </c>
       <c r="E9" s="1">
-        <v>36664</v>
+        <v>38472</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9">
-        <v>40</v>
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
       </c>
       <c r="H9" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="I9" t="s">
         <v>3</v>
       </c>
       <c r="J9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L9" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" t="s">
+        <v>44</v>
+      </c>
+      <c r="N9" t="s">
+        <v>55</v>
+      </c>
+      <c r="O9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="30">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1">
+        <v>36346</v>
+      </c>
+      <c r="E10" s="1">
+        <v>36664</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10">
+        <v>40</v>
+      </c>
+      <c r="H10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L10" t="s">
         <v>38</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="L9" t="s">
-        <v>39</v>
-      </c>
-      <c r="M9" t="s">
-        <v>46</v>
-      </c>
-      <c r="N9" t="s">
-        <v>57</v>
-      </c>
-      <c r="O9" t="b">
+      <c r="M10" t="s">
+        <v>45</v>
+      </c>
+      <c r="N10" t="s">
+        <v>56</v>
+      </c>
+      <c r="O10" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>